<commit_message>
Completed Data visualizing using tableau and added dashboards
</commit_message>
<xml_diff>
--- a/Tableau/world_analysis2.xlsx
+++ b/Tableau/world_analysis2.xlsx
@@ -8,19 +8,32 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/vinaysaireddymandala/Downloads/ML_projects/Covid-Data-Exploration/Tableau/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:9_{664704B4-723D-FA4F-96E7-58A28FD790EC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2CCF4604-20FA-A644-8BCA-148C28A17555}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4340" yWindow="2160" windowWidth="28040" windowHeight="17440" xr2:uid="{13C280D2-7ED8-484F-ABB3-314676BDF1E1}"/>
+    <workbookView xWindow="4320" yWindow="2160" windowWidth="28040" windowHeight="17440" xr2:uid="{13C280D2-7ED8-484F-ABB3-314676BDF1E1}"/>
   </bookViews>
   <sheets>
     <sheet name="Table1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="25">
   <si>
     <t>Location</t>
   </si>
@@ -92,13 +105,16 @@
   </si>
   <si>
     <t>259101</t>
+  </si>
+  <si>
+    <t>Asia</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="18" x14ac:knownFonts="1">
+  <fonts count="19" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -231,6 +247,12 @@
       <color theme="0"/>
       <name val="Aptos Narrow"/>
       <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Aptos Narrow"/>
       <scheme val="minor"/>
     </font>
   </fonts>
@@ -575,8 +597,10 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -952,10 +976,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BC67F7E7-74D5-8044-A9AE-FCC8809A0E6C}">
-  <dimension ref="A1:F7"/>
+  <dimension ref="A1:F8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C13" sqref="C13"/>
+      <selection activeCell="F9" sqref="F9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1108,6 +1132,28 @@
         <v>1.8200000000000001E-2</v>
       </c>
     </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
+        <v>24</v>
+      </c>
+      <c r="B8" s="1">
+        <v>4721383370</v>
+      </c>
+      <c r="C8">
+        <v>301428726</v>
+      </c>
+      <c r="D8">
+        <v>1637060</v>
+      </c>
+      <c r="E8" s="2">
+        <f>(C8/B8)*100</f>
+        <v>6.3843306585798381</v>
+      </c>
+      <c r="F8" s="2">
+        <f>(D8/B8)*100</f>
+        <v>3.4673312283895301E-2</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>